<commit_message>
podzieliłam na tabelki - zaległe
</commit_message>
<xml_diff>
--- a/3 wypadki ogołem z podziałem na przyczyne WOJEWODZTWA.xlsx
+++ b/3 wypadki ogołem z podziałem na przyczyne WOJEWODZTWA.xlsx
@@ -5,15 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repozytoria\AnalizaDanych\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1ADE6E-AA08-416B-AC82-2FA3499B560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43E12AF-D3D7-454E-BFB6-6CE0B4ABF1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TABLICA" sheetId="2" r:id="rId1"/>
+    <sheet name="wina kierowców - ogółem" sheetId="2" r:id="rId1"/>
+    <sheet name="niedostosowanie prędkości" sheetId="3" r:id="rId2"/>
+    <sheet name="nieprzestrzeganie pierwszeństwa" sheetId="4" r:id="rId3"/>
+    <sheet name="nieprawidłowe wyprzedzanie" sheetId="5" r:id="rId4"/>
+    <sheet name="niepraw. zachow. wobec pieszych" sheetId="6" r:id="rId5"/>
+    <sheet name="niebezpieczna odlegość pojazdów" sheetId="7" r:id="rId6"/>
+    <sheet name="wina kierowców - pozostałe" sheetId="8" r:id="rId7"/>
+    <sheet name="wina pieszych - ogółem" sheetId="9" r:id="rId8"/>
+    <sheet name="wina pieszych - niebez. wejście" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -239,7 +247,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -247,6 +255,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -566,7 +577,7 @@
   <dimension ref="A1:BM20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,10 +586,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -664,8 +675,8 @@
       <c r="BM1" s="3"/>
     </row>
     <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
@@ -857,8 +868,8 @@
       </c>
     </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
@@ -4399,19 +4410,117 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="9">
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="Q1:W1"/>
     <mergeCell ref="BG1:BM1"/>
     <mergeCell ref="X1:AD1"/>
     <mergeCell ref="AE1:AK1"/>
     <mergeCell ref="AL1:AR1"/>
     <mergeCell ref="AS1:AY1"/>
     <mergeCell ref="AZ1:BF1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="Q1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03EA1488-23C7-4D33-8BAD-6E6A971EDA33}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC70947-485B-44AD-B0AA-EC150D0260AA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4424BB3-EE12-4BE1-BB78-78F1069E2A0C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC00CCE0-E178-4E0B-8AAA-E99DB0E7E8F7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DAC605-E661-4917-9383-016AC43038D1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2340F5-9E03-4F84-B6FF-FB968920E28C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30CD56DF-5334-43AF-8FA4-1C7E932EBC09}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF9AC821-1246-4E10-B540-D1C681230D44}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>